<commit_message>
Logic and doc update
1. add new logic to check the cases:
TypeToSimpleType - > TypeChange_Update;
TypeToComplexType -> TypeChange_Update.
2. add new samples in SampleAnalysis doc.
</commit_message>
<xml_diff>
--- a/SampleAnalysis.xlsx
+++ b/SampleAnalysis.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
   <si>
     <t>OLD VERSION</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -119,10 +118,6 @@
   </si>
   <si>
     <t>cntc.xsd</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>element name change</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -773,101 +768,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">="Anniversary" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>type="airsyncbase:EmptyTag"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/&gt; -&gt;
-&lt;xs:simpleType name="EmptyTag"&gt;
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;xs:restriction base="xs:string"&gt;
-      &lt;xs:maxLength value="0"/&gt;
-    &lt;/xs:restriction&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-&lt;/xs:simpleType&gt;</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">&lt;xs:element </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>name="Home</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Telephone</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Number" </t>
     </r>
     <r>
       <rPr>
@@ -1860,73 +1760,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">&lt;xs:element </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ref="Home</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Phone</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Number"/&gt; -&gt;
-&lt;xs:element name="HomePhoneNumber" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>type="xs:string"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF3F3F3F"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/&gt;</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">&lt;xs:element name="RecipientCount" type="xs:integer" </t>
     </r>
     <r>
@@ -2063,6 +1896,303 @@
                 this.instanceTypeField = value;
             }
         }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;xs:element name="Children"&gt;
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;xs:complexType&gt;
+            &lt;xs:sequence minOccurs="0"&gt;
+              &lt;xs:element name="Child" type="xs:string" minOccurs="0" maxOccurs="300" /&gt;
+            &lt;/xs:sequence&gt;
+          &lt;/xs:complexType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;/xs:element&gt;</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;xs:element name="Children"&gt;
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;xs:simpleType&gt;
+            &lt;xs:restriction base="xs:string"&gt;
+              &lt;xs:maxLength value="0" /&gt;
+            &lt;/xs:restriction&gt;
+          &lt;/xs:simpleType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;/xs:element&gt;</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexTypeToSimpleType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;xs:element </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ref="Home</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phone</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number"/&gt; -&gt;
+&lt;xs:element name="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Home2PhoneNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type="xs:string"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /&gt;</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Element_NameAttribute_Update
+TypeToSimpleType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;xs:element </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Home2TelephoneNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type="airsyncbase:EmptyTag"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/&gt; -&gt;
+&lt;xs:element name="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Home2TelephoneNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"&gt;
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;xs:simpleType&gt;
+            &lt;xs:restriction base="xs:string"&gt;
+              &lt;xs:maxLength value="0" /&gt;
+            &lt;/xs:restriction&gt;
+          &lt;/xs:simpleType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;/xs:element&gt;</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TypeChange_Update</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2147,7 +2277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2194,6 +2324,17 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2205,7 +2346,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2260,17 +2401,32 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2553,10 +2709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2569,28 +2725,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
@@ -2623,7 +2779,7 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2632,55 +2788,55 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="21"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="21">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
       <c r="E9" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -2696,175 +2852,180 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="21">
         <v>2</v>
       </c>
+      <c r="D11" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="E11" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="13" t="s">
+    </row>
+    <row r="12" spans="1:6" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="18" customFormat="1" ht="108" x14ac:dyDescent="0.15">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="F14" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="21">
+        <v>4</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" ht="366" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5" t="s">
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="17">
-        <v>4</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" ht="366" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="10" t="s">
+    </row>
+    <row r="19" spans="1:6" s="4" customFormat="1" ht="256.5" x14ac:dyDescent="0.15">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="E19" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="256.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="E18" s="7" t="s">
+    </row>
+    <row r="20" spans="1:6" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="E20" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="E19" s="12" t="s">
+      <c r="F20" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>6</v>
@@ -2873,10 +3034,10 @@
     </row>
     <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -2885,112 +3046,112 @@
     </row>
     <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="C29" s="21">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="364.5" x14ac:dyDescent="0.15">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="17">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="364.5" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.15">
-      <c r="A30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -2999,34 +3160,34 @@
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>6</v>
@@ -3035,124 +3196,124 @@
     </row>
     <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="17" t="s">
+    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="17">
+      <c r="C38" s="21">
         <v>1</v>
       </c>
-      <c r="D37" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="D38" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" ht="202.5" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" s="4" customFormat="1" ht="202.5" x14ac:dyDescent="0.15">
+      <c r="A42" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="17">
+      <c r="C42" s="21">
         <v>2</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="D42" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>6</v>
@@ -3161,7 +3322,7 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>86</v>
@@ -3173,10 +3334,10 @@
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -3185,10 +3346,10 @@
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>6</v>
@@ -3197,90 +3358,102 @@
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A49" s="17" t="s">
+    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A50" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="C50" s="21">
+        <v>2</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="17">
-        <v>2</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="E52" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A49:A50"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create data structures and logic for the output of diff result.
</commit_message>
<xml_diff>
--- a/SampleAnalysis.xlsx
+++ b/SampleAnalysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="147">
   <si>
     <t>OLD VERSION</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2451,6 +2451,22 @@
   <si>
     <t>DecreasedMaxOccurs,
 AddMaxOccurs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;xs:element name="OofState"&gt;
+    &lt;xs:simpleType&gt;
+      &lt;xs:restriction base="xs:integer"&gt;
+        &lt;xs:enumeration value="0"/&gt;
+        &lt;xs:enumeration value="1"/&gt;
+        &lt;xs:enumeration value="2"/&gt;
+      &lt;/xs:restriction&gt;
+    &lt;/xs:simpleType&gt;
+  &lt;/xs:element&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>something wrong</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2613,7 +2629,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2674,11 +2690,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2698,17 +2720,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2993,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3007,28 +3032,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
@@ -3061,7 +3086,7 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3070,20 +3095,20 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="21"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
@@ -3095,10 +3120,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="20" t="s">
         <v>144</v>
       </c>
       <c r="E8" s="12" t="s">
@@ -3109,9 +3134,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="E9" s="5" t="s">
         <v>125</v>
       </c>
@@ -3120,9 +3145,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="18" customFormat="1" ht="202.5" x14ac:dyDescent="0.15">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="19" t="s">
         <v>141</v>
       </c>
@@ -3134,9 +3159,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" s="18" customFormat="1" ht="108" x14ac:dyDescent="0.15">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="19" t="s">
         <v>141</v>
       </c>
@@ -3160,13 +3185,13 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="4" t="s">
         <v>137</v>
       </c>
@@ -3178,9 +3203,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="8" t="s">
         <v>135</v>
       </c>
@@ -3192,9 +3217,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" s="17" customFormat="1" ht="108" x14ac:dyDescent="0.15">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="19" t="s">
         <v>133</v>
       </c>
@@ -3236,16 +3261,16 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="21">
         <v>4</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -3256,10 +3281,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" s="14" customFormat="1" ht="366" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="15" t="s">
         <v>130</v>
       </c>
@@ -3268,9 +3293,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="8" t="s">
         <v>31</v>
       </c>
@@ -3282,9 +3307,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1" ht="256.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
       <c r="E21" s="7" t="s">
         <v>113</v>
       </c>
@@ -3293,9 +3318,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
       <c r="E22" s="12" t="s">
         <v>115</v>
       </c>
@@ -3400,13 +3425,13 @@
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="21">
         <v>2</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -3420,9 +3445,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="364.5" x14ac:dyDescent="0.15">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="8" t="s">
         <v>51</v>
       </c>
@@ -3526,16 +3551,16 @@
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="28">
+      <c r="C40" s="21">
         <v>1</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="21" t="s">
         <v>79</v>
       </c>
       <c r="E40" s="5" t="s">
@@ -3546,10 +3571,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
       <c r="E41" s="5" t="s">
         <v>128</v>
       </c>
@@ -3582,13 +3607,13 @@
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:6" s="4" customFormat="1" ht="202.5" x14ac:dyDescent="0.15">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44" s="21">
         <v>2</v>
       </c>
       <c r="D44" s="4" t="s">
@@ -3602,9 +3627,9 @@
       </c>
     </row>
     <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="4" t="s">
         <v>18</v>
       </c>
@@ -3627,7 +3652,7 @@
       </c>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>87</v>
       </c>
@@ -3637,7 +3662,15 @@
       <c r="C47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="D47" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47" s="33" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
@@ -3688,13 +3721,13 @@
       <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:6" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C52" s="28">
+      <c r="C52" s="21">
         <v>2</v>
       </c>
       <c r="E52" s="7" t="s">
@@ -3705,9 +3738,9 @@
       </c>
     </row>
     <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
       <c r="D53" s="4" t="s">
         <v>137</v>
       </c>
@@ -3732,12 +3765,18 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="C18:C22"/>
@@ -3749,18 +3788,12 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>